<commit_message>
motor resolution changed to 0.9°
- before was 1.8°
</commit_message>
<xml_diff>
--- a/calculations/Stepper Motor Resolution.xlsx
+++ b/calculations/Stepper Motor Resolution.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBFC2BE-3F7C-46D1-A99A-2F82ED8287B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="11">
     <numFmt numFmtId="164" formatCode="0.0&quot;°&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0&quot; mm&quot;"/>
@@ -184,7 +185,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -259,6 +260,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -294,6 +312,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,32 +504,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.84375" customWidth="1"/>
+    <col min="5" max="5" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="18.45" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="18.45" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -502,10 +539,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="3">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -514,10 +551,10 @@
       </c>
       <c r="D6">
         <f>360/D5</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -525,13 +562,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="6">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -542,7 +579,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B10" s="20" t="s">
         <v>3</v>
       </c>
@@ -557,7 +594,7 @@
       </c>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B11" s="20"/>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -574,177 +611,177 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" ref="C12:C17" si="0">$D$6*B12</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" ref="D12:D17" si="1">$D$7/C12</f>
-        <v>7.4999999999999997E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E12" s="12">
-        <f>$D$8*D12</f>
-        <v>75</v>
+        <f t="shared" ref="E12:E17" si="2">$D$8*D12</f>
+        <v>50</v>
       </c>
       <c r="F12" s="13">
-        <f t="shared" ref="F12:F17" si="2">E12*60</f>
-        <v>4500</v>
+        <f t="shared" ref="F12:F17" si="3">E12*60</f>
+        <v>3000</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:K17" si="3">C12/$D$7</f>
-        <v>133.33333333333334</v>
+        <f t="shared" ref="K12:K17" si="4">C12/$D$7</f>
+        <v>200</v>
       </c>
       <c r="N12" s="19">
-        <f t="shared" ref="N12:N17" si="4">E12/$D$7*C12</f>
+        <f t="shared" ref="N12:N17" si="5">E12/$D$7*C12</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B13" s="4">
         <v>2</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="1"/>
-        <v>3.7499999999999999E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E13" s="12">
-        <f>$D$8*D13</f>
-        <v>37.5</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="F13" s="13">
-        <f t="shared" si="2"/>
-        <v>2250</v>
+        <f t="shared" si="3"/>
+        <v>1500</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>266.66666666666669</v>
+        <f t="shared" si="4"/>
+        <v>400</v>
       </c>
       <c r="N13" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B14" s="14">
         <v>4</v>
       </c>
       <c r="C14" s="15">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="1"/>
-        <v>1.8749999999999999E-3</v>
+        <v>1.25E-3</v>
       </c>
       <c r="E14" s="17">
-        <f>$D$8*D14</f>
-        <v>18.75</v>
+        <f t="shared" si="2"/>
+        <v>12.5</v>
       </c>
       <c r="F14" s="18">
-        <f t="shared" si="2"/>
-        <v>1125</v>
+        <f t="shared" si="3"/>
+        <v>750</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>533.33333333333337</v>
+        <f t="shared" si="4"/>
+        <v>800</v>
       </c>
       <c r="N14" s="19">
         <f>E14/$D$7*C14</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B15" s="4">
         <v>8</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>3200</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="1"/>
-        <v>9.3749999999999997E-4</v>
+        <v>6.2500000000000001E-4</v>
       </c>
       <c r="E15" s="12">
-        <f>$D$8*D15</f>
-        <v>9.375</v>
+        <f t="shared" si="2"/>
+        <v>6.25</v>
       </c>
       <c r="F15" s="13">
-        <f t="shared" si="2"/>
-        <v>562.5</v>
+        <f t="shared" si="3"/>
+        <v>375</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>1066.6666666666667</v>
+        <f t="shared" si="4"/>
+        <v>1600</v>
       </c>
       <c r="N15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B16" s="4">
         <v>16</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>6400</v>
       </c>
       <c r="D16" s="10">
         <f t="shared" si="1"/>
-        <v>4.6874999999999998E-4</v>
+        <v>3.1250000000000001E-4</v>
       </c>
       <c r="E16" s="12">
-        <f>$D$8*D16</f>
-        <v>4.6875</v>
+        <f t="shared" si="2"/>
+        <v>3.125</v>
       </c>
       <c r="F16" s="13">
-        <f t="shared" si="2"/>
-        <v>281.25</v>
+        <f t="shared" si="3"/>
+        <v>187.5</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
-        <v>2133.3333333333335</v>
+        <f t="shared" si="4"/>
+        <v>3200</v>
       </c>
       <c r="N16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B17" s="4">
         <v>32</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="0"/>
-        <v>6400</v>
+        <v>12800</v>
       </c>
       <c r="D17" s="11">
         <f t="shared" si="1"/>
-        <v>2.3437499999999999E-4</v>
+        <v>1.5625E-4</v>
       </c>
       <c r="E17" s="12">
-        <f>$D$8*D17</f>
-        <v>2.34375</v>
+        <f t="shared" si="2"/>
+        <v>1.5625</v>
       </c>
       <c r="F17" s="13">
-        <f t="shared" si="2"/>
-        <v>140.625</v>
+        <f t="shared" si="3"/>
+        <v>93.75</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
-        <v>4266.666666666667</v>
+        <f t="shared" si="4"/>
+        <v>6400</v>
       </c>
       <c r="N17" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10000</v>
       </c>
     </row>

</xml_diff>